<commit_message>
Error: Productivity Report not generated
</commit_message>
<xml_diff>
--- a/App_Templates/PO_Template.xlsx
+++ b/App_Templates/PO_Template.xlsx
@@ -9,6 +9,9 @@
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">Data!$2:$3</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
@@ -458,10 +461,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="B1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -519,7 +525,10 @@
     <mergeCell ref="F2:F3"/>
     <mergeCell ref="G2:G3"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="90" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>Page &amp;P of &amp;N</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>